<commit_message>
push itération 2 excel
</commit_message>
<xml_diff>
--- a/estimation.xlsx
+++ b/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>implémentation des 10 secondes pour embarquer sur la ligne de tir</t>
+  </si>
+  <si>
+    <t>très peu de travail. Le projet de mi-cession a pris la priorité. Une excuse, mais pas une raison.</t>
   </si>
 </sst>
 </file>
@@ -372,6 +375,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -387,8 +392,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1761,10 +1764,10 @@
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="24"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="11">
         <f>SUM(C16:C21)</f>
         <v>41</v>
@@ -1875,10 +1878,10 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="24"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>49</v>
@@ -2120,10 +2123,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>16</v>
@@ -2150,24 +2153,24 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="27" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="26"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="26"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="26"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="27"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2184,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2253,7 +2256,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="28">
+      <c r="A15" s="23">
         <v>42800</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2264,7 +2267,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+      <c r="A16" s="24">
         <v>42807</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2377,10 +2380,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>7</v>
@@ -2396,7 +2399,9 @@
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
@@ -2405,22 +2410,24 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="26"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="26"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="26"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="27"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2437,7 +2444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
@@ -2610,10 +2617,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2638,22 +2645,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="26"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="26"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="26"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="27"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2843,10 +2850,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2871,22 +2878,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="26"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="26"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="26"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="27"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
push fin de session
</commit_message>
<xml_diff>
--- a/estimation.xlsx
+++ b/estimation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -201,6 +201,21 @@
   </si>
   <si>
     <t>le résultat désiré est obtenu, mais le temps dammandé n'a pas été respecté.</t>
+  </si>
+  <si>
+    <t>travail</t>
+  </si>
+  <si>
+    <t>implémenter les commandes sonores dans l'appli</t>
+  </si>
+  <si>
+    <t>finaliser d'implémenter les commandes sonores dans l'appli</t>
+  </si>
+  <si>
+    <t>apprendre à implémenter des commandes snonres dans une appli</t>
+  </si>
+  <si>
+    <t>création des sonds à implémenter dans l'ap^pli</t>
   </si>
 </sst>
 </file>
@@ -2583,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:B47"/>
+    <sheetView view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2685,17 +2700,23 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="23">
+        <v>42829</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
@@ -2786,7 +2807,7 @@
       <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2844,8 +2865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2902,44 +2923,92 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>42835</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="23">
+        <v>42836</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="23">
+        <v>42842</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="23">
+        <v>42843</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="23">
+        <v>42849</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="23">
+        <v>42850</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="23">
+        <v>42856</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
+      <c r="A21" s="23">
+        <v>42857</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
@@ -3023,7 +3092,7 @@
       <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>